<commit_message>
Continuação da implementação dos detalhes dos aminoácidos.
</commit_message>
<xml_diff>
--- a/aaData/aaData.xlsx
+++ b/aaData/aaData.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="212">
   <si>
     <t>Alanine</t>
   </si>
@@ -53,9 +53,6 @@
     <t>R</t>
   </si>
   <si>
-    <t>Basic polar</t>
-  </si>
-  <si>
     <t>positive</t>
   </si>
   <si>
@@ -297,19 +294,420 @@
   </si>
   <si>
     <t>Aspartate</t>
+  </si>
+  <si>
+    <t>group</t>
+  </si>
+  <si>
+    <t>sideChainGroup</t>
+  </si>
+  <si>
+    <t>molecularMass</t>
+  </si>
+  <si>
+    <t>vanderWaalsV</t>
+  </si>
+  <si>
+    <t>frequency</t>
+  </si>
+  <si>
+    <t>surfaceArea</t>
+  </si>
+  <si>
+    <t>obs</t>
+  </si>
+  <si>
+    <t>methane</t>
+  </si>
+  <si>
+    <t>71.09</t>
+  </si>
+  <si>
+    <t>7.7</t>
+  </si>
+  <si>
+    <t>115</t>
+  </si>
+  <si>
+    <t>Non-polar side chain. Small side chain volume.$Unreactive side chain.</t>
+  </si>
+  <si>
+    <t>electrically charged</t>
+  </si>
+  <si>
+    <t>1-propyl-guanidine</t>
+  </si>
+  <si>
+    <t>basic polar</t>
+  </si>
+  <si>
+    <t>156.19</t>
+  </si>
+  <si>
+    <t>167</t>
+  </si>
+  <si>
+    <t>5.1</t>
+  </si>
+  <si>
+    <t>225</t>
+  </si>
+  <si>
+    <t>Positively charged side chain at pH 7.0. pK for guanidino group in proteins ~12.0.$Participates in ionic interactions with negatively charged groups.</t>
+  </si>
+  <si>
+    <t>polar-neutral</t>
+  </si>
+  <si>
+    <t>acetamide</t>
+  </si>
+  <si>
+    <t>114.11</t>
+  </si>
+  <si>
+    <t>148</t>
+  </si>
+  <si>
+    <t>4.3</t>
+  </si>
+  <si>
+    <t>160</t>
+  </si>
+  <si>
+    <t>Polar, but uncharged, side chain.$Polar side chain will hydrogen bond.$Relatively small side chain volume leads to this residue being found relatively frequently in turns.</t>
+  </si>
+  <si>
+    <t>acetate</t>
+  </si>
+  <si>
+    <t>115.09</t>
+  </si>
+  <si>
+    <t>67</t>
+  </si>
+  <si>
+    <t>5.2</t>
+  </si>
+  <si>
+    <t>150</t>
+  </si>
+  <si>
+    <t>Negatively charged side chain.$pK for side chain of ∼4.0.$Charged side chain exhibits electrostatic interactions with positively charged groups.</t>
+  </si>
+  <si>
+    <t>methanethiol</t>
+  </si>
+  <si>
+    <t>103.15</t>
+  </si>
+  <si>
+    <t>86</t>
+  </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>135</t>
+  </si>
+  <si>
+    <t>Side chain contains thiol (SH) group.$Thiol side chain has pK in isolated amino acid of ~8.5 but in proteins varies 5-10 Thiol group is very reactive</t>
+  </si>
+  <si>
+    <t>propanoate</t>
+  </si>
+  <si>
+    <t>129.12</t>
+  </si>
+  <si>
+    <t>109</t>
+  </si>
+  <si>
+    <t>6.2</t>
+  </si>
+  <si>
+    <t>190</t>
+  </si>
+  <si>
+    <t>Negatively charged side chain.$Side chain has pK of ~4.5.</t>
+  </si>
+  <si>
+    <t>propanamide</t>
+  </si>
+  <si>
+    <t>128.12</t>
+  </si>
+  <si>
+    <t>114</t>
+  </si>
+  <si>
+    <t>4.1</t>
+  </si>
+  <si>
+    <t>180</t>
+  </si>
+  <si>
+    <t>Polar but uncharged side chain.$Polar side chain can hydrogen bond.</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>57.05</t>
+  </si>
+  <si>
+    <t>48</t>
+  </si>
+  <si>
+    <t>7.4</t>
+  </si>
+  <si>
+    <t>75</t>
+  </si>
+  <si>
+    <r>
+      <t>Uncharged, small side chain.$Often found in turn regions of proteins or regions of conformational flexibility.$No chiral centre due to two hydrogens attached to C</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t>α</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> centre</t>
+    </r>
+  </si>
+  <si>
+    <t>4-methyl-1H-imidazole</t>
+  </si>
+  <si>
+    <t>137.14</t>
+  </si>
+  <si>
+    <t>118</t>
+  </si>
+  <si>
+    <t>2.3</t>
+  </si>
+  <si>
+    <t>195</t>
+  </si>
+  <si>
+    <t>Imidazole side chain.$The side chain exhibits a pK ~6.0 in model peptides but in proteins can vary from 4-10.</t>
+  </si>
+  <si>
+    <t>butane</t>
+  </si>
+  <si>
+    <t>113.16</t>
+  </si>
+  <si>
+    <t>124</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>175</t>
+  </si>
+  <si>
+    <t>Hydrophobic side chain exhibiting non-polar based interactions but generally unreactive.$</t>
+  </si>
+  <si>
+    <t>2-methyl-propane</t>
+  </si>
+  <si>
+    <t>8.5</t>
+  </si>
+  <si>
+    <t>170</t>
+  </si>
+  <si>
+    <t>Hydrophobic side chain.</t>
+  </si>
+  <si>
+    <t>butan-1-amine</t>
+  </si>
+  <si>
+    <t>128.17</t>
+  </si>
+  <si>
+    <t>5.9</t>
+  </si>
+  <si>
+    <t>200</t>
+  </si>
+  <si>
+    <t>Positively charged side chain.$Side chain is basic with pK of ~10.5.$Shows ionic interactions.</t>
+  </si>
+  <si>
+    <t>(methyl-sulfanyl)ethane</t>
+  </si>
+  <si>
+    <t>131.19</t>
+  </si>
+  <si>
+    <t>2.4</t>
+  </si>
+  <si>
+    <t>185</t>
+  </si>
+  <si>
+    <t>Sulfur containing hydrophobic side chain.$ The sulfur is unreactive especially when compared with thiol group of cysteine.</t>
+  </si>
+  <si>
+    <t>aromatic</t>
+  </si>
+  <si>
+    <t>methyl-benzene</t>
+  </si>
+  <si>
+    <t>147.18</t>
+  </si>
+  <si>
+    <t>4.0</t>
+  </si>
+  <si>
+    <t>210</t>
+  </si>
+  <si>
+    <t>Hydrophobic, aromatic side chain.$Phenyl ring is chemically unreactive in proteins.$Exhibits weak optical absorbance around 280nm.</t>
+  </si>
+  <si>
+    <t>pyrrolidine</t>
+  </si>
+  <si>
+    <t>97.12</t>
+  </si>
+  <si>
+    <t>90</t>
+  </si>
+  <si>
+    <t>145</t>
+  </si>
+  <si>
+    <t>Cyclic ring forming hydrophobic side chain.$The cyclic ring limits conformational flexibility around N-Cα bond.$In a polypeptide chain lacks amide hydrogen and cannot form backbone hydrogen bonds.</t>
+  </si>
+  <si>
+    <t>methanol</t>
+  </si>
+  <si>
+    <t>87.08</t>
+  </si>
+  <si>
+    <t>73</t>
+  </si>
+  <si>
+    <t>6.9</t>
+  </si>
+  <si>
+    <t>Polar but uncharged side chain.$Contains hydroxyl group (-OH) that hydrogen bonds.$Oxygen atom can act as potent nucleophile in some enzymes.</t>
+  </si>
+  <si>
+    <t>ethanol</t>
+  </si>
+  <si>
+    <t>101.11</t>
+  </si>
+  <si>
+    <t>93</t>
+  </si>
+  <si>
+    <t>140</t>
+  </si>
+  <si>
+    <t>Polar but uncharged side chain.$Contains hydroxyl group (-OH).$Hydrogen bonding side chain</t>
+  </si>
+  <si>
+    <t>3-methyl-1H-indole</t>
+  </si>
+  <si>
+    <t>186.21</t>
+  </si>
+  <si>
+    <t>163</t>
+  </si>
+  <si>
+    <t>1.4</t>
+  </si>
+  <si>
+    <t>255</t>
+  </si>
+  <si>
+    <t>Large, hydrophobic and aromatic side chain.$Almost all reactivity is based around the indole ring nitrogen.$Responsible for majority of near uv absorbance in proteins at 280nm.</t>
+  </si>
+  <si>
+    <t>4-methyl-phenol</t>
+  </si>
+  <si>
+    <t>163.18</t>
+  </si>
+  <si>
+    <t>141</t>
+  </si>
+  <si>
+    <t>3.2</t>
+  </si>
+  <si>
+    <t>230</t>
+  </si>
+  <si>
+    <t>Aromatic side chain. Phenolic hydroxyl group ionizes at pH values around pH 10.$Aromatic ring more easily substituted than that of phenylalanine.</t>
+  </si>
+  <si>
+    <t>propane</t>
+  </si>
+  <si>
+    <t>99.14</t>
+  </si>
+  <si>
+    <t>105</t>
+  </si>
+  <si>
+    <t>6.6</t>
+  </si>
+  <si>
+    <t>155</t>
+  </si>
+  <si>
+    <t>Hydrophobic side chain</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -332,9 +730,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -615,42 +1014,71 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="J28" sqref="J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="3" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="28.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.5703125" customWidth="1"/>
+    <col min="11" max="11" width="10" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="183" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>72</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>77</v>
-      </c>
-      <c r="D1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="H1" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I1" s="2" t="s">
+        <v>92</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>93</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="M1" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -664,13 +1092,34 @@
         <v>3</v>
       </c>
       <c r="E2" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="1" t="s">
+      <c r="H2" s="1" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>6</v>
       </c>
@@ -681,376 +1130,778 @@
         <v>8</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="H3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="B4" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" s="1" t="s">
+      <c r="I4" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>117</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="M6" s="1" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C7" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="J7" s="1" t="s">
+        <v>131</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>133</v>
+      </c>
+      <c r="M7" s="1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D4" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C5" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A7" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="C7" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C8" s="1" t="s">
+      <c r="H8" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="J8" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="L8" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="M8" s="1" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="D8" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
+      <c r="B9" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="C9" s="1" t="s">
         <v>29</v>
-      </c>
-      <c r="C9" s="1" t="s">
-        <v>30</v>
       </c>
       <c r="D9" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="I9" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J9" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L9" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="M9" s="1" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="H10" s="1" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A10" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="1" t="s">
+      <c r="I10" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="J10" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="L10" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="M10" s="1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D10" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="F10" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A11" s="1" t="s">
+      <c r="B11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B11" s="1" t="s">
+      <c r="C11" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>36</v>
       </c>
       <c r="D11" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="F11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G11" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="H11" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>156</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A12" s="1" t="s">
+      <c r="B12" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="1" t="s">
+      <c r="C12" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="D12" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I12" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="J12" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="L12" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="M12" s="1" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A13" s="1" t="s">
+      <c r="B13" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="B13" s="1" t="s">
+      <c r="C13" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="D13" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I13" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="J13" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L13" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="M13" s="1" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="D13" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="F13" s="1" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="B14" s="1" t="s">
+      <c r="C14" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="D14" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="F14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="H14" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="K14" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="L14" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="M14" s="1" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A15" s="1" t="s">
         <v>48</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A15" s="1" t="s">
+      <c r="B15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B15" s="1" t="s">
+      <c r="C15" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C15" s="1" t="s">
+      <c r="D15" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H15" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="D15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E15" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="1" t="s">
+      <c r="I15" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="K15" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="L15" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="M15" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A16" s="1" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A16" s="1" t="s">
+      <c r="B16" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="B16" s="1" t="s">
+      <c r="C16" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C16" s="1" t="s">
-        <v>55</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="H16" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="K16" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="L16" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="M16" s="1" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="H17" s="1" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A17" s="1" t="s">
-        <v>56</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="C17" s="1" t="s">
+      <c r="I17" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="J17" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="K17" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="L17" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="M17" s="1" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D17" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E17" s="1" t="s">
+      <c r="B18" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H18" s="1" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A18" s="1" t="s">
-        <v>59</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="C18" s="1" t="s">
+      <c r="I18" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="J18" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="K18" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="L18" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="M18" s="1" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E18" s="1" t="s">
+      <c r="B19" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="F19" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="H19" s="1" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A19" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="C19" s="1" t="s">
+      <c r="I19" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="J19" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="K19" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="L19" s="1" t="s">
+        <v>198</v>
+      </c>
+      <c r="M19" s="1" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="D19" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="E19" s="1" t="s">
+      <c r="B20" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>200</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="H20" s="1" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A20" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>66</v>
-      </c>
-      <c r="C20" s="1" t="s">
+      <c r="I20" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="J20" s="1" t="s">
+        <v>202</v>
+      </c>
+      <c r="K20" s="1" t="s">
+        <v>203</v>
+      </c>
+      <c r="L20" s="1" t="s">
+        <v>204</v>
+      </c>
+      <c r="M20" s="1" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="D20" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="1" t="s">
+      <c r="B21" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B21" s="1" t="s">
+      <c r="C21" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="D21" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="G21" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>71</v>
+      <c r="H21" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="I21" s="1" t="s">
+        <v>207</v>
+      </c>
+      <c r="J21" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="K21" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="L21" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="M21" s="1" t="s">
+        <v>211</v>
       </c>
     </row>
   </sheetData>
+  <sortState ref="A2:M21">
+    <sortCondition ref="A1"/>
+  </sortState>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>

</xml_diff>